<commit_message>
Org type, flow date type, new formatted columns
</commit_message>
<xml_diff>
--- a/output/Congo, The Democratic Republic of the_aggregated.xlsx
+++ b/output/Congo, The Democratic Republic of the_aggregated.xlsx
@@ -20,43 +20,151 @@
     <t xml:space="preserve">amountUSD</t>
   </si>
   <si>
+    <t xml:space="preserve">United States of America, Government of</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Central Emergency Response Fund</t>
+  </si>
+  <si>
+    <t xml:space="preserve">European Commission's Humanitarian Aid and Civil Protection Department</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Democratic Republic of the Congo Humanitarian Fund</t>
+  </si>
+  <si>
+    <t xml:space="preserve">World Bank</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Japan, Government of</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Canada, Government of</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ireland, Government of</t>
+  </si>
+  <si>
     <t xml:space="preserve">Germany, Government of</t>
   </si>
   <si>
-    <t xml:space="preserve">United States of America, Government of</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Canada, Government of</t>
-  </si>
-  <si>
-    <t xml:space="preserve">European Commission's Humanitarian Aid and Civil Protection Department</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Central Emergency Response Fund</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ireland, Government of</t>
+    <t xml:space="preserve">France, Government of</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Luxembourg, Government of</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Denmark, Government of</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Netherlands, Government of</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Norway, Government of</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sweden, Government of</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Paul G. Allen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US Fund for UNICEF</t>
+  </si>
+  <si>
+    <t xml:space="preserve"/>
+  </si>
+  <si>
+    <t xml:space="preserve">United Nations Children's Fund</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNICEF National Committee/Netherlands</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNICEF National Committee/Belgium</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNICEF National Committee/Japan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNICEF National Committee/France</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNICEF National Committee/Germany</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Belgium, Government of</t>
+  </si>
+  <si>
+    <t xml:space="preserve">United Kingdom, Government of</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Private (individuals &amp; organizations)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPS Foundation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNICEF National Committee/United Kingdom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Switzerland, Government of</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNICEF National Committee/Denmark</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jersey Overseas Aid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Liechtenstein, Government of</t>
   </si>
   <si>
     <t xml:space="preserve">Italy, Government of</t>
   </si>
   <si>
-    <t xml:space="preserve">Sweden, Government of</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Denmark, Government of</t>
+    <t xml:space="preserve">World Health Organization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">World Food Programme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Congo, Democratic Republic of, Government of</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Finland, Government of</t>
   </si>
   <si>
     <t xml:space="preserve">United Nations Population Fund</t>
   </si>
   <si>
-    <t xml:space="preserve">World Bank</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Luxembourg, Government of</t>
-  </si>
-  <si>
-    <t xml:space="preserve">United Kingdom, Government of</t>
+    <t xml:space="preserve">Korea, Republic of, Government of</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Women's Refugee Commission</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mercy Corps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Austria, Government of</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spain, Government of</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Malta, Government of</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Office for the Coordination of Humanitarian Affairs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UN Programme on HIV/AIDS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">United Nations High Commissioner for Refugees</t>
+  </si>
+  <si>
+    <t xml:space="preserve">European Commission EuropeAid Development and Cooperation</t>
   </si>
   <si>
     <t xml:space="preserve">GAVI Alliance</t>
@@ -65,121 +173,13 @@
     <t xml:space="preserve">WELLCOME TRUST</t>
   </si>
   <si>
-    <t xml:space="preserve">Norway, Government of</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US Fund for UNICEF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Switzerland, Government of</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spain, Government of</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Belgium, Government of</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mercy Corps</t>
-  </si>
-  <si>
-    <t xml:space="preserve"/>
-  </si>
-  <si>
-    <t xml:space="preserve">United Nations Children's Fund</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Malta, Government of</t>
+    <t xml:space="preserve">Bill and Melinda Gates Foundation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UN Peacebuilding Fund</t>
   </si>
   <si>
     <t xml:space="preserve">United Nations Foundation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Austria, Government of</t>
-  </si>
-  <si>
-    <t xml:space="preserve">France, Government of</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Office for the Coordination of Humanitarian Affairs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Private (individuals &amp; organizations)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UN Programme on HIV/AIDS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Japan, Government of</t>
-  </si>
-  <si>
-    <t xml:space="preserve">World Health Organization</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UNICEF National Committee/Netherlands</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UNICEF National Committee/Belgium</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UNICEF National Committee/Japan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UNICEF National Committee/France</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UNICEF National Committee/Germany</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Democratic Republic of the Congo Humanitarian Fund</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Liechtenstein, Government of</t>
-  </si>
-  <si>
-    <t xml:space="preserve">World Food Programme</t>
-  </si>
-  <si>
-    <t xml:space="preserve">United Nations High Commissioner for Refugees</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPS Foundation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Finland, Government of</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UN Peacebuilding Fund</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Korea, Republic of, Government of</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UNICEF National Committee/United Kingdom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bill and Melinda Gates Foundation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jersey Overseas Aid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Women's Refugee Commission</t>
-  </si>
-  <si>
-    <t xml:space="preserve">European Commission EuropeAid Development and Cooperation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Netherlands, Government of</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UNICEF National Committee/Denmark</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Congo, Democratic Republic of, Government of</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Paul G. Allen</t>
   </si>
 </sst>
 </file>
@@ -524,7 +524,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>163399161</v>
+        <v>903803816</v>
       </c>
     </row>
     <row r="3">
@@ -532,7 +532,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>903803816</v>
+        <v>56218866</v>
       </c>
     </row>
     <row r="4">
@@ -540,7 +540,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>30068666</v>
+        <v>98852207</v>
       </c>
     </row>
     <row r="5">
@@ -548,7 +548,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="n">
-        <v>98852207</v>
+        <v>79707195</v>
       </c>
     </row>
     <row r="6">
@@ -556,7 +556,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="n">
-        <v>56218866</v>
+        <v>42649999</v>
       </c>
     </row>
     <row r="7">
@@ -564,7 +564,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="n">
-        <v>12854014</v>
+        <v>11090236</v>
       </c>
     </row>
     <row r="8">
@@ -572,7 +572,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="n">
-        <v>3556838</v>
+        <v>30068666</v>
       </c>
     </row>
     <row r="9">
@@ -580,7 +580,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="n">
-        <v>46637746</v>
+        <v>12854014</v>
       </c>
     </row>
     <row r="10">
@@ -588,7 +588,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="n">
-        <v>7509149</v>
+        <v>163399161</v>
       </c>
     </row>
     <row r="11">
@@ -596,7 +596,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="n">
-        <v>1507325</v>
+        <v>8299224</v>
       </c>
     </row>
     <row r="12">
@@ -604,7 +604,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="n">
-        <v>42649999</v>
+        <v>2842767</v>
       </c>
     </row>
     <row r="13">
@@ -612,7 +612,7 @@
         <v>13</v>
       </c>
       <c r="B13" t="n">
-        <v>2842767</v>
+        <v>7509149</v>
       </c>
     </row>
     <row r="14">
@@ -620,7 +620,7 @@
         <v>14</v>
       </c>
       <c r="B14" t="n">
-        <v>220376763</v>
+        <v>24914099</v>
       </c>
     </row>
     <row r="15">
@@ -628,7 +628,7 @@
         <v>15</v>
       </c>
       <c r="B15" t="n">
-        <v>1000000</v>
+        <v>23958352</v>
       </c>
     </row>
     <row r="16">
@@ -636,7 +636,7 @@
         <v>16</v>
       </c>
       <c r="B16" t="n">
-        <v>4132050</v>
+        <v>46637746</v>
       </c>
     </row>
     <row r="17">
@@ -644,7 +644,7 @@
         <v>17</v>
       </c>
       <c r="B17" t="n">
-        <v>23958352</v>
+        <v>3894094</v>
       </c>
     </row>
     <row r="18">
@@ -660,7 +660,7 @@
         <v>19</v>
       </c>
       <c r="B19" t="n">
-        <v>19450665</v>
+        <v>15230092</v>
       </c>
     </row>
     <row r="20">
@@ -668,7 +668,7 @@
         <v>20</v>
       </c>
       <c r="B20" t="n">
-        <v>837027</v>
+        <v>46662132</v>
       </c>
     </row>
     <row r="21">
@@ -676,7 +676,7 @@
         <v>21</v>
       </c>
       <c r="B21" t="n">
-        <v>27553160</v>
+        <v>40509</v>
       </c>
     </row>
     <row r="22">
@@ -684,7 +684,7 @@
         <v>22</v>
       </c>
       <c r="B22" t="n">
-        <v>857449</v>
+        <v>165720</v>
       </c>
     </row>
     <row r="23">
@@ -692,7 +692,7 @@
         <v>23</v>
       </c>
       <c r="B23" t="n">
-        <v>15230092</v>
+        <v>61194</v>
       </c>
     </row>
     <row r="24">
@@ -700,7 +700,7 @@
         <v>24</v>
       </c>
       <c r="B24" t="n">
-        <v>46662132</v>
+        <v>873014</v>
       </c>
     </row>
     <row r="25">
@@ -708,7 +708,7 @@
         <v>25</v>
       </c>
       <c r="B25" t="n">
-        <v>29481</v>
+        <v>1596929</v>
       </c>
     </row>
     <row r="26">
@@ -716,7 +716,7 @@
         <v>26</v>
       </c>
       <c r="B26" t="n">
-        <v>887</v>
+        <v>27553160</v>
       </c>
     </row>
     <row r="27">
@@ -724,7 +724,7 @@
         <v>27</v>
       </c>
       <c r="B27" t="n">
-        <v>115741</v>
+        <v>220376763</v>
       </c>
     </row>
     <row r="28">
@@ -732,7 +732,7 @@
         <v>28</v>
       </c>
       <c r="B28" t="n">
-        <v>8299224</v>
+        <v>2917862</v>
       </c>
     </row>
     <row r="29">
@@ -740,7 +740,7 @@
         <v>29</v>
       </c>
       <c r="B29" t="n">
-        <v>3649679</v>
+        <v>321001</v>
       </c>
     </row>
     <row r="30">
@@ -748,7 +748,7 @@
         <v>30</v>
       </c>
       <c r="B30" t="n">
-        <v>2917862</v>
+        <v>1905601</v>
       </c>
     </row>
     <row r="31">
@@ -756,7 +756,7 @@
         <v>31</v>
       </c>
       <c r="B31" t="n">
-        <v>85000</v>
+        <v>19450665</v>
       </c>
     </row>
     <row r="32">
@@ -764,7 +764,7 @@
         <v>32</v>
       </c>
       <c r="B32" t="n">
-        <v>11090236</v>
+        <v>254644</v>
       </c>
     </row>
     <row r="33">
@@ -772,7 +772,7 @@
         <v>33</v>
       </c>
       <c r="B33" t="n">
-        <v>880792</v>
+        <v>544487</v>
       </c>
     </row>
     <row r="34">
@@ -780,7 +780,7 @@
         <v>34</v>
       </c>
       <c r="B34" t="n">
-        <v>40509</v>
+        <v>201310</v>
       </c>
     </row>
     <row r="35">
@@ -788,7 +788,7 @@
         <v>35</v>
       </c>
       <c r="B35" t="n">
-        <v>165720</v>
+        <v>3556838</v>
       </c>
     </row>
     <row r="36">
@@ -796,7 +796,7 @@
         <v>36</v>
       </c>
       <c r="B36" t="n">
-        <v>61194</v>
+        <v>880792</v>
       </c>
     </row>
     <row r="37">
@@ -804,7 +804,7 @@
         <v>37</v>
       </c>
       <c r="B37" t="n">
-        <v>873014</v>
+        <v>10808469</v>
       </c>
     </row>
     <row r="38">
@@ -812,7 +812,7 @@
         <v>38</v>
       </c>
       <c r="B38" t="n">
-        <v>1596929</v>
+        <v>5146451</v>
       </c>
     </row>
     <row r="39">
@@ -820,7 +820,7 @@
         <v>39</v>
       </c>
       <c r="B39" t="n">
-        <v>79707195</v>
+        <v>4277948</v>
       </c>
     </row>
     <row r="40">
@@ -828,7 +828,7 @@
         <v>40</v>
       </c>
       <c r="B40" t="n">
-        <v>201310</v>
+        <v>1507325</v>
       </c>
     </row>
     <row r="41">
@@ -836,7 +836,7 @@
         <v>41</v>
       </c>
       <c r="B41" t="n">
-        <v>10808469</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="42">
@@ -844,7 +844,7 @@
         <v>42</v>
       </c>
       <c r="B42" t="n">
-        <v>1142857</v>
+        <v>110057</v>
       </c>
     </row>
     <row r="43">
@@ -852,7 +852,7 @@
         <v>43</v>
       </c>
       <c r="B43" t="n">
-        <v>321001</v>
+        <v>857449</v>
       </c>
     </row>
     <row r="44">
@@ -860,7 +860,7 @@
         <v>44</v>
       </c>
       <c r="B44" t="n">
-        <v>4277948</v>
+        <v>115741</v>
       </c>
     </row>
     <row r="45">
@@ -868,7 +868,7 @@
         <v>45</v>
       </c>
       <c r="B45" t="n">
-        <v>399990</v>
+        <v>837027</v>
       </c>
     </row>
     <row r="46">
@@ -876,7 +876,7 @@
         <v>46</v>
       </c>
       <c r="B46" t="n">
-        <v>200000</v>
+        <v>29481</v>
       </c>
     </row>
     <row r="47">
@@ -884,7 +884,7 @@
         <v>47</v>
       </c>
       <c r="B47" t="n">
-        <v>1905601</v>
+        <v>3649679</v>
       </c>
     </row>
     <row r="48">
@@ -892,7 +892,7 @@
         <v>48</v>
       </c>
       <c r="B48" t="n">
-        <v>4000000</v>
+        <v>85000</v>
       </c>
     </row>
     <row r="49">
@@ -900,7 +900,7 @@
         <v>49</v>
       </c>
       <c r="B49" t="n">
-        <v>544487</v>
+        <v>1142857</v>
       </c>
     </row>
     <row r="50">
@@ -908,7 +908,7 @@
         <v>50</v>
       </c>
       <c r="B50" t="n">
-        <v>110057</v>
+        <v>3184475</v>
       </c>
     </row>
     <row r="51">
@@ -916,7 +916,7 @@
         <v>51</v>
       </c>
       <c r="B51" t="n">
-        <v>3184475</v>
+        <v>1000000</v>
       </c>
     </row>
     <row r="52">
@@ -924,7 +924,7 @@
         <v>52</v>
       </c>
       <c r="B52" t="n">
-        <v>24914099</v>
+        <v>4132050</v>
       </c>
     </row>
     <row r="53">
@@ -932,7 +932,7 @@
         <v>53</v>
       </c>
       <c r="B53" t="n">
-        <v>254644</v>
+        <v>4000000</v>
       </c>
     </row>
     <row r="54">
@@ -940,7 +940,7 @@
         <v>54</v>
       </c>
       <c r="B54" t="n">
-        <v>5146451</v>
+        <v>399990</v>
       </c>
     </row>
     <row r="55">
@@ -948,7 +948,7 @@
         <v>55</v>
       </c>
       <c r="B55" t="n">
-        <v>3894094</v>
+        <v>887</v>
       </c>
     </row>
   </sheetData>

</xml_diff>